<commit_message>
Adding light mode diagrams and updating minutes
</commit_message>
<xml_diff>
--- a/Requirements/Group 1 Meeting Minutes.xlsx
+++ b/Requirements/Group 1 Meeting Minutes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/orion/Desktop/School/Fall_2023/Software_engineering/Comms-Project/Requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5FAFC16-B19B-E14E-A0EE-279A0AB953FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A674679-93B7-FD4F-8615-CA2422C9F28B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="26960" windowHeight="22400" xr2:uid="{2F142419-51C2-2041-A355-CBD947EA1066}"/>
+    <workbookView xWindow="38400" yWindow="500" windowWidth="32140" windowHeight="22400" xr2:uid="{2F142419-51C2-2041-A355-CBD947EA1066}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>CS401 Group 1 Meeting Minutes</t>
   </si>
@@ -111,6 +111,21 @@
   </si>
   <si>
     <t>Sedat, David, Madison, Sean, Joseph</t>
+  </si>
+  <si>
+    <t>October 14 2023</t>
+  </si>
+  <si>
+    <t>6:00PM</t>
+  </si>
+  <si>
+    <t>User sends a message -&gt; sent to the server -&gt; writes to room file</t>
+  </si>
+  <si>
+    <t>7:05PM</t>
+  </si>
+  <si>
+    <t>Redid use case diagram</t>
   </si>
 </sst>
 </file>
@@ -177,11 +192,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -500,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA31A564-7EC9-D245-B573-18204F8350BD}">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -513,19 +527,19 @@
     <col min="3" max="3" width="16.6640625" customWidth="1"/>
     <col min="4" max="4" width="14.5" customWidth="1"/>
     <col min="5" max="5" width="68.5" customWidth="1"/>
-    <col min="6" max="6" width="23.33203125" customWidth="1"/>
+    <col min="6" max="6" width="53.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="59" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="59" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -541,89 +555,96 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B9" s="4"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adding updating meeting minutes
</commit_message>
<xml_diff>
--- a/Requirements/Group 1 Meeting Minutes.xlsx
+++ b/Requirements/Group 1 Meeting Minutes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/orion/Desktop/School/Fall_2023/Software_engineering/Comms-Project/Requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A674679-93B7-FD4F-8615-CA2422C9F28B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D10C5B2E-CF84-1B4A-87DC-8664E3FADD0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="500" windowWidth="32140" windowHeight="22400" xr2:uid="{2F142419-51C2-2041-A355-CBD947EA1066}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="30620" windowHeight="20780" xr2:uid="{2F142419-51C2-2041-A355-CBD947EA1066}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>CS401 Group 1 Meeting Minutes</t>
   </si>
@@ -126,6 +126,15 @@
   </si>
   <si>
     <t>Redid use case diagram</t>
+  </si>
+  <si>
+    <t>October 15 2023</t>
+  </si>
+  <si>
+    <t>7:00PM</t>
+  </si>
+  <si>
+    <t>Sedat, Madison, Joseph, David</t>
   </si>
 </sst>
 </file>
@@ -517,7 +526,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -526,7 +535,7 @@
     <col min="2" max="2" width="34.6640625" customWidth="1"/>
     <col min="3" max="3" width="16.6640625" customWidth="1"/>
     <col min="4" max="4" width="14.5" customWidth="1"/>
-    <col min="5" max="5" width="68.5" customWidth="1"/>
+    <col min="5" max="5" width="69.6640625" customWidth="1"/>
     <col min="6" max="6" width="53.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -644,7 +653,15 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B10" s="3"/>
+      <c r="A10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updating the meeting minutes
</commit_message>
<xml_diff>
--- a/Requirements/Group 1 Meeting Minutes.xlsx
+++ b/Requirements/Group 1 Meeting Minutes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/orion/Desktop/School/Fall_2023/Software_engineering/Comms-Project/Requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D10C5B2E-CF84-1B4A-87DC-8664E3FADD0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413B6AE0-B5A8-DE4F-B7F9-C927BCBAB22A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="30620" windowHeight="20780" xr2:uid="{2F142419-51C2-2041-A355-CBD947EA1066}"/>
   </bookViews>
@@ -134,7 +134,7 @@
     <t>7:00PM</t>
   </si>
   <si>
-    <t>Sedat, Madison, Joseph, David</t>
+    <t>Sedat, Madison, Joseph, David, Sean</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
New meetingMinutes and adding to the Gantt Chart
</commit_message>
<xml_diff>
--- a/Requirements/Group 1 Meeting Minutes.xlsx
+++ b/Requirements/Group 1 Meeting Minutes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/orion/Desktop/School/Fall_2023/Software_engineering/Comms-Project/Requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413B6AE0-B5A8-DE4F-B7F9-C927BCBAB22A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D2748B3-DEA7-7F49-92AF-8637D70B0B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="30620" windowHeight="20780" xr2:uid="{2F142419-51C2-2041-A355-CBD947EA1066}"/>
+    <workbookView xWindow="2400" yWindow="1080" windowWidth="30620" windowHeight="20780" xr2:uid="{2F142419-51C2-2041-A355-CBD947EA1066}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
   <si>
     <t>CS401 Group 1 Meeting Minutes</t>
   </si>
@@ -135,6 +135,24 @@
   </si>
   <si>
     <t>Sedat, Madison, Joseph, David, Sean</t>
+  </si>
+  <si>
+    <t>October 21 2023</t>
+  </si>
+  <si>
+    <t>7:10PM</t>
+  </si>
+  <si>
+    <t>8:00PM</t>
+  </si>
+  <si>
+    <t>Finish up Presentation Slides</t>
+  </si>
+  <si>
+    <t>Figuring out what are we supposed to do next in the project</t>
+  </si>
+  <si>
+    <t>8:35PM</t>
   </si>
 </sst>
 </file>
@@ -523,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA31A564-7EC9-D245-B573-18204F8350BD}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -662,6 +680,29 @@
       <c r="C10" s="6" t="s">
         <v>31</v>
       </c>
+      <c r="D10" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>37</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updaing files from meeting
</commit_message>
<xml_diff>
--- a/Requirements/Group 1 Meeting Minutes.xlsx
+++ b/Requirements/Group 1 Meeting Minutes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/orion/Desktop/School/Fall_2023/Software_engineering/Comms-Project/Requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D390FBD-87D8-8645-8CEC-A3CE66B42B05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE90DC0-2E2E-E541-AE7D-C2195D97F1D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2400" yWindow="1080" windowWidth="30620" windowHeight="20780" xr2:uid="{2F142419-51C2-2041-A355-CBD947EA1066}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
   <si>
     <t>CS401 Group 1 Meeting Minutes</t>
   </si>
@@ -159,6 +159,15 @@
   </si>
   <si>
     <t>Sedat, Madison, Sean</t>
+  </si>
+  <si>
+    <t>9:30PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chatrooms UID are based off of the users in the room (it is created when the first message is sent), User ID are based on the first letter of the first name and the first letter of their last name followed by 5 digits </t>
+  </si>
+  <si>
+    <t>Worked on Presentation slides and class diagram - Adding Structure of Presentation</t>
   </si>
 </sst>
 </file>
@@ -559,7 +568,7 @@
     <col min="2" max="2" width="34.6640625" customWidth="1"/>
     <col min="3" max="3" width="16.6640625" customWidth="1"/>
     <col min="4" max="4" width="14.5" customWidth="1"/>
-    <col min="5" max="5" width="69.6640625" customWidth="1"/>
+    <col min="5" max="5" width="83.83203125" customWidth="1"/>
     <col min="6" max="6" width="53.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -720,6 +729,15 @@
       <c r="C12" s="6" t="s">
         <v>31</v>
       </c>
+      <c r="D12" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
final design phase additions
</commit_message>
<xml_diff>
--- a/Requirements/Group 1 Meeting Minutes.xlsx
+++ b/Requirements/Group 1 Meeting Minutes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/orion/Desktop/School/Fall_2023/Software_engineering/Comms-Project/Requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C17D80DE-7F04-4548-A5C7-CDB66C689B4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{672847E3-CBDB-B143-91C2-D59E13739AB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="22460" windowHeight="22380" xr2:uid="{2F142419-51C2-2041-A355-CBD947EA1066}"/>
+    <workbookView xWindow="14000" yWindow="500" windowWidth="21540" windowHeight="21560" xr2:uid="{2F142419-51C2-2041-A355-CBD947EA1066}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
   <si>
     <t>CS401 Group 1 Meeting Minutes</t>
   </si>
@@ -177,6 +177,12 @@
   </si>
   <si>
     <t>Finish up Presentation Slides for Design</t>
+  </si>
+  <si>
+    <t>November 2 2023</t>
+  </si>
+  <si>
+    <t>Madison</t>
   </si>
 </sst>
 </file>
@@ -565,10 +571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA31A564-7EC9-D245-B573-18204F8350BD}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="108" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -765,6 +771,17 @@
         <v>46</v>
       </c>
     </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
adding to the minutes
</commit_message>
<xml_diff>
--- a/Requirements/Group 1 Meeting Minutes.xlsx
+++ b/Requirements/Group 1 Meeting Minutes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/orion/Desktop/School/Fall_2023/Software_engineering/Comms-Project/Requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{672847E3-CBDB-B143-91C2-D59E13739AB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B8D67D-1CA5-1947-BED6-66E747159023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14000" yWindow="500" windowWidth="21540" windowHeight="21560" xr2:uid="{2F142419-51C2-2041-A355-CBD947EA1066}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="51">
   <si>
     <t>CS401 Group 1 Meeting Minutes</t>
   </si>
@@ -182,7 +182,13 @@
     <t>November 2 2023</t>
   </si>
   <si>
-    <t>Madison</t>
+    <t>November 16 2023</t>
+  </si>
+  <si>
+    <t>1:15PM</t>
+  </si>
+  <si>
+    <t>Worked on the java files of application</t>
   </si>
 </sst>
 </file>
@@ -571,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA31A564-7EC9-D245-B573-18204F8350BD}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="108" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -775,12 +781,27 @@
       <c r="A14" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>48</v>
-      </c>
+      <c r="B14" s="3"/>
       <c r="C14" s="6" t="s">
         <v>31</v>
       </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E16" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adding updated meeting minutes
</commit_message>
<xml_diff>
--- a/Requirements/Group 1 Meeting Minutes.xlsx
+++ b/Requirements/Group 1 Meeting Minutes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/orion/Desktop/School/Fall_2023/Software_engineering/Comms-Project/Requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B8D67D-1CA5-1947-BED6-66E747159023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F4E09D-CFC2-A94C-9F71-FD8662DCBBB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14000" yWindow="500" windowWidth="21540" windowHeight="21560" xr2:uid="{2F142419-51C2-2041-A355-CBD947EA1066}"/>
+    <workbookView xWindow="5780" yWindow="500" windowWidth="26360" windowHeight="21560" xr2:uid="{2F142419-51C2-2041-A355-CBD947EA1066}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="56">
   <si>
     <t>CS401 Group 1 Meeting Minutes</t>
   </si>
@@ -189,6 +189,21 @@
   </si>
   <si>
     <t>Worked on the java files of application</t>
+  </si>
+  <si>
+    <t>November 18 2023</t>
+  </si>
+  <si>
+    <t>2:00PM</t>
+  </si>
+  <si>
+    <t>2:45PM</t>
+  </si>
+  <si>
+    <t>2:15PM</t>
+  </si>
+  <si>
+    <t>Update each other on what was done and what needs to be done going forwards</t>
   </si>
 </sst>
 </file>
@@ -579,8 +594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA31A564-7EC9-D245-B573-18204F8350BD}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="108" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -796,12 +811,29 @@
       <c r="C15" s="6" t="s">
         <v>49</v>
       </c>
+      <c r="D15" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="E15" s="3" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E16" s="3"/>
+      <c r="A16" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>55</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>